<commit_message>
ups for real this time
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/PVPUmp_Data_tabs.xlsx
+++ b/heliostrome/jip_project/results/PVPUmp_Data_tabs.xlsx
@@ -33,7 +33,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,13 +43,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -104,10 +98,10 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -12220,7 +12214,7 @@
     <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12228,7 +12222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1">
         <v>25569.04211056713</v>
       </c>
@@ -12236,7 +12230,7 @@
         <v>1.610704453977936</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1">
         <v>25569.042110578703</v>
       </c>
@@ -12244,7 +12238,7 @@
         <v>1.665894451867128</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1">
         <v>25569.04211059028</v>
       </c>
@@ -12252,7 +12246,7 @@
         <v>1.17773128533068</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1">
         <v>25569.04211060185</v>
       </c>
@@ -12260,7 +12254,7 @@
         <v>1.49031666958615</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1">
         <v>25569.042110613427</v>
       </c>
@@ -12268,7 +12262,7 @@
         <v>1.56269404112251</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1">
         <v>25569.042110625</v>
       </c>
@@ -12276,7 +12270,7 @@
         <v>1.572296187624942</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1">
         <v>25569.042110636576</v>
       </c>
@@ -12284,7 +12278,7 @@
         <v>0.8067263419202717</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1">
         <v>25569.042110648148</v>
       </c>
@@ -12292,7 +12286,7 @@
         <v>1.42956841765088</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1">
         <v>25569.04211065972</v>
       </c>
@@ -12300,7 +12294,7 @@
         <v>0.6167889680203195</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1">
         <v>25569.042110671297</v>
       </c>
@@ -12308,7 +12302,7 @@
         <v>0.3498147629260526</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1">
         <v>25569.04211068287</v>
       </c>
@@ -12316,7 +12310,7 @@
         <v>0.9537476512652607</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1">
         <v>25569.042110694445</v>
       </c>
@@ -12324,7 +12318,7 @@
         <v>1.672528834398547</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1">
         <v>25569.042110706017</v>
       </c>
@@ -12332,7 +12326,7 @@
         <v>1.698167293784765</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1">
         <v>25569.042110717593</v>
       </c>
@@ -12340,7 +12334,7 @@
         <v>1.791470345848534</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1">
         <v>25569.042110729166</v>
       </c>
@@ -12348,7 +12342,7 @@
         <v>1.742452857923113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1">
         <v>25569.042110740742</v>
       </c>
@@ -12356,7 +12350,7 @@
         <v>1.743269720335346</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1">
         <v>25569.042110752314</v>
       </c>

</xml_diff>